<commit_message>
remove 62.2 from datalist
</commit_message>
<xml_diff>
--- a/datalists/N2_40_g_list.xlsx
+++ b/datalists/N2_40_g_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>/data2/shared/data/twoColour/Results/recording51/recording51.3g100-250/recording51.3g_X1_skeletons.hdf5</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>/data2/shared/data/twoColour/Results/recording61/recording61.2g100-250/recording61.2g_X1_skeletons.hdf5</t>
-  </si>
-  <si>
-    <t>/data2/shared/data/twoColour/Results/recording62/recording62.2g100-250/recording62.2g_X1_skeletons.hdf5</t>
   </si>
 </sst>
 </file>
@@ -99,6 +96,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="69.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -173,12 +173,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>19440.0</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
remove 62.2 from datalist due to bad compression (#10)
* adapt correlation analysis to for phase restriction, untested, commit before pulling from master

* commit before pulling

* phase-specific correlation function ready to be tested. create figures/correlation/phaseSpecific folder before testing so figures can be saved accordingly

* add script to plot distribution of turn features

* update analysis to include phase restriction to multiple scripts, including for N2 movies

* add 1W turn figures

* modify turnFeatures.m to compare cluster leaving vs lone worms

* rename plotTurnFeatures.m

* remove 62.2 from datalist
</commit_message>
<xml_diff>
--- a/datalists/N2_40_g_list.xlsx
+++ b/datalists/N2_40_g_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>/data2/shared/data/twoColour/Results/recording51/recording51.3g100-250/recording51.3g_X1_skeletons.hdf5</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>/data2/shared/data/twoColour/Results/recording61/recording61.2g100-250/recording61.2g_X1_skeletons.hdf5</t>
-  </si>
-  <si>
-    <t>/data2/shared/data/twoColour/Results/recording62/recording62.2g100-250/recording62.2g_X1_skeletons.hdf5</t>
   </si>
 </sst>
 </file>
@@ -99,6 +96,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="69.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -173,12 +173,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>19440.0</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
modify turn analysis and in cluster proportion to include multiple phase restriction options
</commit_message>
<xml_diff>
--- a/datalists/N2_40_g_list.xlsx
+++ b/datalists/N2_40_g_list.xlsx
@@ -105,7 +105,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="2">
@@ -113,7 +122,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="3">
@@ -121,7 +139,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="4">
@@ -129,7 +156,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="5">
@@ -137,7 +173,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="6">
@@ -145,7 +190,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="7">
@@ -153,7 +207,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="8">
@@ -161,7 +224,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="9">
@@ -169,7 +241,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>19440.0</v>
+        <v>10044.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>19440.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20412.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32400.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>